<commit_message>
Added github link in spec doc
</commit_message>
<xml_diff>
--- a/specification_doc_learner's_academy.xlsx
+++ b/specification_doc_learner's_academy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Learner's Academy App Version-1</t>
   </si>
@@ -30,9 +30,6 @@
     <t>*The application has two parts:One for data upload to MySQL database and the other part is for report generation.</t>
   </si>
   <si>
-    <t>Brief Description:The project uses Servlets,JSP,MySQL databse server and Hibernate to implement the specific details.</t>
-  </si>
-  <si>
     <t>*The admin logs in by providing the right credentials and is then directed to a page which provides the features to upload data and view the reports.</t>
   </si>
   <si>
@@ -130,6 +127,37 @@
   </si>
   <si>
     <t>On hitting the Get Master Report button</t>
+  </si>
+  <si>
+    <t>GitHubLink</t>
+  </si>
+  <si>
+    <t>https://github.com/Priyam777/LearnersAcademyApp_Priyadarshi_Panigrahi.git</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Brief Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:The project uses Servlets,JSP,MySQL databse server and Hibernate to implement the specific details.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -181,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -207,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -217,6 +251,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,13 +270,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5572125</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -279,13 +317,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3219450</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -326,13 +364,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8315325</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -373,13 +411,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -420,13 +458,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7038975</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -467,13 +505,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7267575</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -514,13 +552,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3333750</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -561,13 +599,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7115175</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>171</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -608,13 +646,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6429375</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -655,13 +693,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5591175</xdr:colOff>
-      <xdr:row>202</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -702,13 +740,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>208</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5619750</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -749,13 +787,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295650</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -796,13 +834,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>237</xdr:row>
+      <xdr:row>241</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6877050</xdr:colOff>
-      <xdr:row>264</xdr:row>
+      <xdr:row>268</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -843,13 +881,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>265</xdr:row>
+      <xdr:row>269</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6296025</xdr:colOff>
-      <xdr:row>280</xdr:row>
+      <xdr:row>284</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -890,13 +928,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>284</xdr:row>
+      <xdr:row>288</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7486650</xdr:colOff>
-      <xdr:row>293</xdr:row>
+      <xdr:row>297</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -937,13 +975,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>295</xdr:row>
+      <xdr:row>299</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7105650</xdr:colOff>
-      <xdr:row>305</xdr:row>
+      <xdr:row>309</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -984,13 +1022,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>308</xdr:row>
+      <xdr:row>312</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3219450</xdr:colOff>
-      <xdr:row>326</xdr:row>
+      <xdr:row>330</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1031,13 +1069,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>329</xdr:row>
+      <xdr:row>333</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7696200</xdr:colOff>
-      <xdr:row>355</xdr:row>
+      <xdr:row>359</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1078,13 +1116,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>356</xdr:row>
+      <xdr:row>360</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3695700</xdr:colOff>
-      <xdr:row>361</xdr:row>
+      <xdr:row>365</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1125,13 +1163,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>365</xdr:row>
+      <xdr:row>369</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7372350</xdr:colOff>
-      <xdr:row>373</xdr:row>
+      <xdr:row>377</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1172,13 +1210,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>375</xdr:row>
+      <xdr:row>379</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7696200</xdr:colOff>
-      <xdr:row>384</xdr:row>
+      <xdr:row>388</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1219,13 +1257,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>387</xdr:row>
+      <xdr:row>391</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3276600</xdr:colOff>
-      <xdr:row>400</xdr:row>
+      <xdr:row>404</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1266,13 +1304,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>402</xdr:row>
+      <xdr:row>406</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7448550</xdr:colOff>
-      <xdr:row>428</xdr:row>
+      <xdr:row>432</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1313,13 +1351,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>429</xdr:row>
+      <xdr:row>433</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3200400</xdr:colOff>
-      <xdr:row>434</xdr:row>
+      <xdr:row>438</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1360,13 +1398,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>438</xdr:row>
+      <xdr:row>442</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7572375</xdr:colOff>
-      <xdr:row>448</xdr:row>
+      <xdr:row>452</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1407,13 +1445,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>451</xdr:row>
+      <xdr:row>455</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7486650</xdr:colOff>
-      <xdr:row>462</xdr:row>
+      <xdr:row>466</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1454,13 +1492,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>465</xdr:row>
+      <xdr:row>469</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3276600</xdr:colOff>
-      <xdr:row>483</xdr:row>
+      <xdr:row>487</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1501,13 +1539,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>485</xdr:row>
+      <xdr:row>489</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7391400</xdr:colOff>
-      <xdr:row>511</xdr:row>
+      <xdr:row>515</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1548,13 +1586,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>513</xdr:row>
+      <xdr:row>517</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7715250</xdr:colOff>
-      <xdr:row>539</xdr:row>
+      <xdr:row>543</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1595,13 +1633,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>543</xdr:row>
+      <xdr:row>547</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7048500</xdr:colOff>
-      <xdr:row>554</xdr:row>
+      <xdr:row>558</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1642,13 +1680,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>556</xdr:row>
+      <xdr:row>560</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7553325</xdr:colOff>
-      <xdr:row>568</xdr:row>
+      <xdr:row>572</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1689,13 +1727,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>571</xdr:row>
+      <xdr:row>575</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3228975</xdr:colOff>
-      <xdr:row>589</xdr:row>
+      <xdr:row>593</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1736,13 +1774,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>591</xdr:row>
+      <xdr:row>595</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8153400</xdr:colOff>
-      <xdr:row>618</xdr:row>
+      <xdr:row>622</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1783,13 +1821,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>619</xdr:row>
+      <xdr:row>623</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8382000</xdr:colOff>
-      <xdr:row>645</xdr:row>
+      <xdr:row>649</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1830,13 +1868,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>646</xdr:row>
+      <xdr:row>650</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4381500</xdr:colOff>
-      <xdr:row>656</xdr:row>
+      <xdr:row>660</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1877,13 +1915,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>664</xdr:row>
+      <xdr:row>668</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7877175</xdr:colOff>
-      <xdr:row>689</xdr:row>
+      <xdr:row>693</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1924,13 +1962,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>692</xdr:row>
+      <xdr:row>696</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3362325</xdr:colOff>
-      <xdr:row>712</xdr:row>
+      <xdr:row>716</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1971,13 +2009,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>714</xdr:row>
+      <xdr:row>718</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7153275</xdr:colOff>
-      <xdr:row>741</xdr:row>
+      <xdr:row>745</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2018,13 +2056,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>745</xdr:row>
+      <xdr:row>749</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5295900</xdr:colOff>
-      <xdr:row>771</xdr:row>
+      <xdr:row>775</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2065,13 +2103,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>774</xdr:row>
+      <xdr:row>778</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3333750</xdr:colOff>
-      <xdr:row>798</xdr:row>
+      <xdr:row>802</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2112,13 +2150,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>801</xdr:row>
+      <xdr:row>805</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7248525</xdr:colOff>
-      <xdr:row>828</xdr:row>
+      <xdr:row>832</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2159,13 +2197,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>829</xdr:row>
+      <xdr:row>833</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3000375</xdr:colOff>
-      <xdr:row>832</xdr:row>
+      <xdr:row>836</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2206,13 +2244,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>837</xdr:row>
+      <xdr:row>841</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7286625</xdr:colOff>
-      <xdr:row>862</xdr:row>
+      <xdr:row>866</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2253,13 +2291,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>865</xdr:row>
+      <xdr:row>869</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6905625</xdr:colOff>
-      <xdr:row>892</xdr:row>
+      <xdr:row>896</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2300,13 +2338,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>893</xdr:row>
+      <xdr:row>897</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2695575</xdr:colOff>
-      <xdr:row>896</xdr:row>
+      <xdr:row>900</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2347,13 +2385,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>902</xdr:row>
+      <xdr:row>906</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7296150</xdr:colOff>
-      <xdr:row>920</xdr:row>
+      <xdr:row>924</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2394,13 +2432,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>924</xdr:row>
+      <xdr:row>928</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3228975</xdr:colOff>
-      <xdr:row>938</xdr:row>
+      <xdr:row>942</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2441,13 +2479,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>941</xdr:row>
+      <xdr:row>945</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7029450</xdr:colOff>
-      <xdr:row>967</xdr:row>
+      <xdr:row>971</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2488,13 +2526,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>968</xdr:row>
+      <xdr:row>972</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2286000</xdr:colOff>
-      <xdr:row>972</xdr:row>
+      <xdr:row>976</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2535,13 +2573,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>977</xdr:row>
+      <xdr:row>981</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7191375</xdr:colOff>
-      <xdr:row>994</xdr:row>
+      <xdr:row>998</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2582,13 +2620,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>997</xdr:row>
+      <xdr:row>1001</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>7153275</xdr:colOff>
-      <xdr:row>1023</xdr:row>
+      <xdr:row>1027</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2629,13 +2667,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1025</xdr:row>
+      <xdr:row>1029</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6772275</xdr:colOff>
-      <xdr:row>1052</xdr:row>
+      <xdr:row>1056</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2676,13 +2714,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1053</xdr:row>
+      <xdr:row>1057</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4581525</xdr:colOff>
-      <xdr:row>1066</xdr:row>
+      <xdr:row>1070</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2723,13 +2761,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1067</xdr:row>
+      <xdr:row>1071</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8353425</xdr:colOff>
-      <xdr:row>1094</xdr:row>
+      <xdr:row>1098</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2770,13 +2808,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1095</xdr:row>
+      <xdr:row>1099</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2019300</xdr:colOff>
-      <xdr:row>1098</xdr:row>
+      <xdr:row>1102</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2817,13 +2855,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1099</xdr:row>
+      <xdr:row>1103</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8486775</xdr:colOff>
-      <xdr:row>1126</xdr:row>
+      <xdr:row>1130</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2864,13 +2902,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1127</xdr:row>
+      <xdr:row>1131</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2162175</xdr:colOff>
-      <xdr:row>1130</xdr:row>
+      <xdr:row>1134</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3195,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1025"/>
+  <dimension ref="A1:A1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1107" workbookViewId="0">
-      <selection activeCell="A1128" sqref="A1128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3221,313 +3259,327 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="5" spans="1:1" s="9" customFormat="1"/>
+    <row r="6" spans="1:1" s="12" customFormat="1">
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="10" customFormat="1">
+      <c r="A7" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="12" customFormat="1">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="6" customFormat="1">
+      <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="6" customFormat="1">
-      <c r="A8" s="6" t="s">
+    <row r="14" spans="1:1" s="1" customFormat="1">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="1" customFormat="1">
-      <c r="A10" s="1" t="s">
+    <row r="15" spans="1:1" s="4" customFormat="1">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="4" customFormat="1">
-      <c r="A11" s="4" t="s">
+    <row r="24" spans="1:1" s="4" customFormat="1">
+      <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="4" customFormat="1">
-      <c r="A20" s="4" t="s">
+    <row r="39" spans="1:1" s="4" customFormat="1">
+      <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="4" customFormat="1">
-      <c r="A35" s="4" t="s">
+    <row r="65" spans="1:1" s="1" customFormat="1">
+      <c r="A65" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:1" s="1" customFormat="1">
-      <c r="A61" s="1" t="s">
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" s="1" customFormat="1">
+      <c r="A95" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" s="1" customFormat="1">
-      <c r="A91" s="1" t="s">
+    <row r="96" spans="1:1" s="4" customFormat="1">
+      <c r="A96" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" s="4" customFormat="1">
+      <c r="A107" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:1" s="4" customFormat="1">
-      <c r="A92" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" s="4" customFormat="1">
-      <c r="A103" s="4" t="s">
+    <row r="119" spans="1:1" s="4" customFormat="1">
+      <c r="A119" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:1" s="4" customFormat="1">
-      <c r="A115" s="4" t="s">
+    <row r="144" spans="1:1" s="4" customFormat="1">
+      <c r="A144" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" s="1" customFormat="1">
+      <c r="A196" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:1" s="4" customFormat="1">
-      <c r="A140" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" s="1" customFormat="1">
-      <c r="A192" s="1" t="s">
+    <row r="197" spans="1:1" s="4" customFormat="1">
+      <c r="A197" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" s="4" customFormat="1">
+      <c r="A208" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="193" spans="1:1" s="4" customFormat="1">
-      <c r="A193" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" s="4" customFormat="1">
-      <c r="A204" s="4" t="s">
+    <row r="221" spans="1:1" s="4" customFormat="1">
+      <c r="A221" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="227" s="4" customFormat="1"/>
+    <row r="228" s="4" customFormat="1"/>
+    <row r="229" s="4" customFormat="1"/>
+    <row r="230" s="4" customFormat="1"/>
+    <row r="231" s="4" customFormat="1"/>
+    <row r="232" s="4" customFormat="1"/>
+    <row r="233" s="4" customFormat="1"/>
+    <row r="234" s="4" customFormat="1"/>
+    <row r="235" s="4" customFormat="1"/>
+    <row r="236" s="4" customFormat="1"/>
+    <row r="237" s="4" customFormat="1"/>
+    <row r="238" s="4" customFormat="1"/>
+    <row r="239" s="4" customFormat="1"/>
+    <row r="240" s="4" customFormat="1"/>
+    <row r="241" spans="1:1" s="4" customFormat="1">
+      <c r="A241" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" s="1" customFormat="1">
+      <c r="A287" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:1" s="4" customFormat="1">
-      <c r="A217" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" s="4" customFormat="1"/>
-    <row r="224" spans="1:1" s="4" customFormat="1"/>
-    <row r="225" spans="1:1" s="4" customFormat="1"/>
-    <row r="226" spans="1:1" s="4" customFormat="1"/>
-    <row r="227" spans="1:1" s="4" customFormat="1"/>
-    <row r="228" spans="1:1" s="4" customFormat="1"/>
-    <row r="229" spans="1:1" s="4" customFormat="1"/>
-    <row r="230" spans="1:1" s="4" customFormat="1"/>
-    <row r="231" spans="1:1" s="4" customFormat="1"/>
-    <row r="232" spans="1:1" s="4" customFormat="1"/>
-    <row r="233" spans="1:1" s="4" customFormat="1"/>
-    <row r="234" spans="1:1" s="4" customFormat="1"/>
-    <row r="235" spans="1:1" s="4" customFormat="1"/>
-    <row r="236" spans="1:1" s="4" customFormat="1"/>
-    <row r="237" spans="1:1" s="4" customFormat="1">
-      <c r="A237" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" s="1" customFormat="1">
-      <c r="A283" s="1" t="s">
+    <row r="288" spans="1:1" s="4" customFormat="1">
+      <c r="A288" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" s="4" customFormat="1">
+      <c r="A299" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="284" spans="1:1" s="4" customFormat="1">
-      <c r="A284" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" s="4" customFormat="1">
-      <c r="A295" s="4" t="s">
+    <row r="312" spans="1:1" s="4" customFormat="1">
+      <c r="A312" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:1" s="4" customFormat="1">
-      <c r="A308" s="4" t="s">
+    <row r="332" spans="1:1" s="4" customFormat="1">
+      <c r="A332" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" s="8" customFormat="1">
+      <c r="A368" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="328" spans="1:1" s="4" customFormat="1">
-      <c r="A328" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="364" spans="1:1" s="8" customFormat="1">
-      <c r="A364" s="8" t="s">
+    <row r="369" spans="1:1" s="4" customFormat="1">
+      <c r="A369" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" s="4" customFormat="1">
+      <c r="A379" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="365" spans="1:1" s="4" customFormat="1">
-      <c r="A365" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="375" spans="1:1" s="4" customFormat="1">
-      <c r="A375" s="4" t="s">
+    <row r="391" spans="1:1" s="4" customFormat="1">
+      <c r="A391" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" s="4" customFormat="1">
+      <c r="A406" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" s="8" customFormat="1">
+      <c r="A441" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="387" spans="1:1" s="4" customFormat="1">
-      <c r="A387" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="402" spans="1:1" s="4" customFormat="1">
-      <c r="A402" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="437" spans="1:1" s="8" customFormat="1">
-      <c r="A437" s="8" t="s">
+    <row r="442" spans="1:1" s="7" customFormat="1">
+      <c r="A442" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" s="4" customFormat="1">
+      <c r="A455" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="438" spans="1:1" s="7" customFormat="1">
-      <c r="A438" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="451" spans="1:1" s="4" customFormat="1">
-      <c r="A451" s="4" t="s">
+    <row r="469" spans="1:1" s="4" customFormat="1">
+      <c r="A469" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" s="4" customFormat="1">
+      <c r="A489" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" s="8" customFormat="1">
+      <c r="A546" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="465" spans="1:1" s="4" customFormat="1">
-      <c r="A465" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="485" spans="1:1" s="4" customFormat="1">
-      <c r="A485" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="542" spans="1:1" s="8" customFormat="1">
-      <c r="A542" s="8" t="s">
+    <row r="547" spans="1:1" s="4" customFormat="1">
+      <c r="A547" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" s="4" customFormat="1">
+      <c r="A560" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="543" spans="1:1" s="4" customFormat="1">
-      <c r="A543" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="556" spans="1:1" s="4" customFormat="1">
-      <c r="A556" s="4" t="s">
+    <row r="575" spans="1:1" s="4" customFormat="1">
+      <c r="A575" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" s="4" customFormat="1">
+      <c r="A595" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="571" spans="1:1" s="4" customFormat="1">
-      <c r="A571" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="591" spans="1:1" s="4" customFormat="1">
-      <c r="A591" s="4" t="s">
+    <row r="663" spans="1:1" s="8" customFormat="1">
+      <c r="A663" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="659" spans="1:1" s="8" customFormat="1">
-      <c r="A659" s="8" t="s">
+    <row r="665" spans="1:1" s="8" customFormat="1">
+      <c r="A665" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="661" spans="1:1" s="8" customFormat="1">
-      <c r="A661" s="8" t="s">
+    <row r="667" spans="1:1" s="4" customFormat="1">
+      <c r="A667" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="663" spans="1:1" s="4" customFormat="1">
-      <c r="A663" s="4" t="s">
+    <row r="695" spans="1:1" s="4" customFormat="1">
+      <c r="A695" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1" s="4" customFormat="1">
+      <c r="A718" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="747" spans="1:1" s="8" customFormat="1">
+      <c r="A747" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="691" spans="1:1" s="4" customFormat="1">
-      <c r="A691" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="714" spans="1:1" s="4" customFormat="1">
-      <c r="A714" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="743" spans="1:1" s="8" customFormat="1">
-      <c r="A743" s="8" t="s">
+    <row r="749" spans="1:1" s="4" customFormat="1">
+      <c r="A749" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="745" spans="1:1" s="4" customFormat="1">
-      <c r="A745" s="4" t="s">
+    <row r="778" spans="1:1" s="4" customFormat="1">
+      <c r="A778" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1" s="4" customFormat="1">
+      <c r="A804" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="839" spans="1:1" s="8" customFormat="1">
+      <c r="A839" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="774" spans="1:1" s="4" customFormat="1">
-      <c r="A774" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="800" spans="1:1" s="4" customFormat="1">
-      <c r="A800" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="835" spans="1:1" s="8" customFormat="1">
-      <c r="A835" s="8" t="s">
+    <row r="841" spans="1:1" s="4" customFormat="1">
+      <c r="A841" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="837" spans="1:1" s="4" customFormat="1">
-      <c r="A837" s="4" t="s">
+    <row r="869" spans="1:1" s="4" customFormat="1">
+      <c r="A869" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="903" spans="1:1" s="8" customFormat="1">
+      <c r="A903" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="865" spans="1:1" s="4" customFormat="1">
-      <c r="A865" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="899" spans="1:1" s="8" customFormat="1">
-      <c r="A899" s="8" t="s">
+    <row r="905" spans="1:1" s="4" customFormat="1">
+      <c r="A905" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="901" spans="1:1" s="4" customFormat="1">
-      <c r="A901" s="4" t="s">
+    <row r="927" spans="1:1" s="4" customFormat="1">
+      <c r="A927" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="944" spans="1:1" s="4" customFormat="1">
+      <c r="A944" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="978" spans="1:1" s="8" customFormat="1">
+      <c r="A978" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="923" spans="1:1" s="4" customFormat="1">
-      <c r="A923" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="940" spans="1:1" s="4" customFormat="1">
-      <c r="A940" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="974" spans="1:1" s="8" customFormat="1">
-      <c r="A974" s="8" t="s">
+    <row r="980" spans="1:1" s="4" customFormat="1">
+      <c r="A980" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="976" spans="1:1" s="4" customFormat="1">
-      <c r="A976" s="4" t="s">
+    <row r="1000" spans="1:1" s="4" customFormat="1">
+      <c r="A1000" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="996" spans="1:1" s="4" customFormat="1">
-      <c r="A996" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:1" s="4" customFormat="1">
-      <c r="A1025" s="4" t="s">
-        <v>9</v>
+    <row r="1029" spans="1:1" s="4" customFormat="1">
+      <c r="A1029" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>